<commit_message>
Excel data writing class
</commit_message>
<xml_diff>
--- a/VytrackTestUsers.xlsx
+++ b/VytrackTestUsers.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3926" uniqueCount="1480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3929" uniqueCount="1483">
   <si>
     <t>username</t>
   </si>
@@ -4476,6 +4476,15 @@
   </si>
   <si>
     <t>SKIPPED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Date of execution</t>
+  </si>
+  <si>
+    <t>2020-04-14T19:18:33.753376</t>
   </si>
 </sst>
 </file>
@@ -18244,7 +18253,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C30F00C-C683-0548-B7C4-02FB1EBCAEF1}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -18276,6 +18285,9 @@
       <c r="F1" t="s">
         <v>1476</v>
       </c>
+      <c r="G1" t="s">
+        <v>1481</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -18294,7 +18306,10 @@
         <v>305</v>
       </c>
       <c r="F2" t="s">
-        <v>1478</v>
+        <v>1480</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1482</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>